<commit_message>
latest batch number... added total range entry in production test sth protocol
</commit_message>
<xml_diff>
--- a/ProductionTests/Sthv2.1.9.xlsx
+++ b/ProductionTests/Sthv2.1.9.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>BBCB4862</t>
+          <t>BBCB4863</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>-50.043487548828125</t>
+          <t>-49.36293411254883</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>-0.035588379949331284</t>
+          <t>-0.005451507400721312</t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>

</xml_diff>

<commit_message>
New STH Limits module integrated everywhere STU Limits module new and integrated
</commit_message>
<xml_diff>
--- a/ProductionTests/Sthv2.1.9.xlsx
+++ b/ProductionTests/Sthv2.1.9.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>BBCB4863</t>
+          <t>D20-4889</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>20191209</t>
+          <t>20191210</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>-49.36293411254883</t>
+          <t>-50.440223693847656</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>-0.005451507400721312</t>
+          <t>-0.03243118152022362</t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>

</xml_diff>

<commit_message>
Minor adaptions inc batch number STH  Bluetooth address test for STU and Sth better file naming
</commit_message>
<xml_diff>
--- a/ProductionTests/Sthv2.1.9.xlsx
+++ b/ProductionTests/Sthv2.1.9.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>D20-4889</t>
+          <t>BBCB4866</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1124,7 +1124,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>20191210</t>
+          <t>20191212</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>98</t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -1417,6 +1417,13 @@
       <c r="H8" s="2" t="inlineStr">
         <is>
           <t>Consecutive number for manufactured devices</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>9259266508322</t>
         </is>
       </c>
     </row>
@@ -1510,7 +1517,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>0.0015259021893143654</t>
+          <t>0.0030518043786287308</t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
@@ -1544,7 +1551,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>-50.440223693847656</t>
+          <t>-99.06767272949219</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1748,7 +1755,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>-0.03243118152022362</t>
+          <t>-0.051661375910043716</t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>

</xml_diff>

<commit_message>
new SSTH batch number Sth limits changed:  iAdcAccXTolerance from 3 to 3,5  uSamplingTolerance from +-10% to +-3% Adaption of run time to determine correct sampling rate test0516AdcOverSamplingRateMax compared with +-10% because of only 220 samples/s correction of limits(auto replace problem) -> raw vs SI-limit
</commit_message>
<xml_diff>
--- a/ProductionTests/Sthv2.1.9.xlsx
+++ b/ProductionTests/Sthv2.1.9.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>BBCB4866</t>
+          <t>BBCB4859</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>20191212</t>
+          <t>20191213</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>106</t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -1423,7 +1423,7 @@
     <row r="9">
       <c r="E9" t="inlineStr">
         <is>
-          <t>9259266508322</t>
+          <t>9259266512513</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>-99.06767272949219</t>
+          <t>-102.89463806152344</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>-0.051661375910043716</t>
+          <t>-0.04075469821691513</t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>

</xml_diff>